<commit_message>
Adjust comment for Power_WeightsK (-> v0.1.4)
Reorder some functions and definitions alphabetically
</commit_message>
<xml_diff>
--- a/data/example/Power_WeightsK.xlsx
+++ b/data/example/Power_WeightsK.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioA" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ScenarioB" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ScenarioA" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="ScenarioB" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -590,7 +590,7 @@
   <cols>
     <col width="5.5709375" customWidth="1" min="1" max="1"/>
     <col width="19.7109375" customWidth="1" min="2" max="2"/>
-    <col width="15.7109375" customWidth="1" min="3" max="3"/>
+    <col width="17.7109375" customWidth="1" min="3" max="3"/>
     <col width="31.7109375" customWidth="1" min="4" max="4"/>
     <col width="24.5709375" customWidth="1" min="5" max="5"/>
     <col width="24.5709375" customWidth="1" min="6" max="6"/>
@@ -616,7 +616,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.3</t>
+          <t>v0.1.4</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Representative hour within rp</t>
+          <t>Representative time step within rp</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">
@@ -1333,7 +1333,7 @@
   <cols>
     <col width="5.5709375" customWidth="1" min="1" max="1"/>
     <col width="19.7109375" customWidth="1" min="2" max="2"/>
-    <col width="15.7109375" customWidth="1" min="3" max="3"/>
+    <col width="17.7109375" customWidth="1" min="3" max="3"/>
     <col width="31.7109375" customWidth="1" min="4" max="4"/>
     <col width="24.5709375" customWidth="1" min="5" max="5"/>
     <col width="24.5709375" customWidth="1" min="6" max="6"/>
@@ -1359,7 +1359,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.1.3</t>
+          <t>v0.1.4</t>
         </is>
       </c>
     </row>
@@ -1425,7 +1425,7 @@
       </c>
       <c r="C5" s="7" t="inlineStr">
         <is>
-          <t>Representative hour within rp</t>
+          <t>Representative time step within rp</t>
         </is>
       </c>
       <c r="D5" s="7" t="inlineStr">

</xml_diff>